<commit_message>
Ajout Burn Down Chart Sprint 0
Ajout Burn Down Chart Sprint 0 = conception et architecture
</commit_message>
<xml_diff>
--- a/ProxiV4 - Product backlog.xlsx
+++ b/ProxiV4 - Product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="29295" windowHeight="14475" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="29295" windowHeight="14475" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -1490,6 +1490,1153 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Burn Down Chart Sprint 0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Points d'effort optimaux</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$34:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Points d'effort réalisés</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$33:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="240187200"/>
+        <c:axId val="239308624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="240187200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="239308624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="239308624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Points d'effort</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="240187200"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1831,7 +2978,7 @@
   <dimension ref="B2:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C29"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -2326,7 +3473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2703,30 +3850,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B19:B25"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2736,8 +3883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3713,6 +4860,7 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Ajout Taches user stories
</commit_message>
<xml_diff>
--- a/ProxiV4 - Product backlog.xlsx
+++ b/ProxiV4 - Product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="29295" windowHeight="14475" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="29295" windowHeight="14475" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -2608,16 +2608,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2977,8 +2977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -3473,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -3883,8 +3883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Mise a jour PB
</commit_message>
<xml_diff>
--- a/ProxiV4 - Product backlog.xlsx
+++ b/ProxiV4 - Product backlog.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminl\Desktop\Rob\depot git\ProxiBanqueV4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="29295" windowHeight="14475" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25700" yWindow="0" windowWidth="29300" windowHeight="17180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="tâches" sheetId="3" r:id="rId2"/>
+    <sheet name="tâches User Stories" sheetId="3" r:id="rId2"/>
     <sheet name="Sprint 0" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -157,9 +152,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>10h00</t>
-  </si>
-  <si>
     <t>12h00</t>
   </si>
   <si>
@@ -262,15 +254,6 @@
     <t>09h00</t>
   </si>
   <si>
-    <t>11h00</t>
-  </si>
-  <si>
-    <t>13h00</t>
-  </si>
-  <si>
-    <t>14h00</t>
-  </si>
-  <si>
     <t>Product Owner</t>
   </si>
   <si>
@@ -404,6 +387,18 @@
   </si>
   <si>
     <t>3) afficher la page d'acceuil du conseiller</t>
+  </si>
+  <si>
+    <t>10h30</t>
+  </si>
+  <si>
+    <t>13h30</t>
+  </si>
+  <si>
+    <t>15h00</t>
+  </si>
+  <si>
+    <t>16h30</t>
   </si>
 </sst>
 </file>
@@ -414,7 +409,7 @@
     <numFmt numFmtId="164" formatCode="ddd\ dd/mm"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -887,41 +882,41 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1259,14 +1254,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -1495,7 +1490,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1541,26 +1536,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1605,25 +1580,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1635,25 +1610,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>111</c:v>
+                  <c:v>111.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74</c:v>
+                  <c:v>74.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,25 +1672,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,25 +1702,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>111.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1762,11 +1737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="240187200"/>
-        <c:axId val="239308624"/>
+        <c:axId val="-2096667832"/>
+        <c:axId val="-2131276376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240187200"/>
+        <c:axId val="-2096667832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,26 +1782,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1862,10 +1817,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239308624"/>
+        <c:crossAx val="-2131276376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1873,7 +1828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239308624"/>
+        <c:axId val="-2131276376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1928,26 +1883,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1977,11 +1912,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240187200"/>
-        <c:crossesAt val="1"/>
+        <c:crossAx val="-2096667832"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2020,7 +1955,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2050,7 +1985,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2981,18 +2916,18 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="3" max="3" width="62.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="16.5" thickBot="1"/>
+    <row r="2" spans="2:12" ht="16" thickBot="1"/>
     <row r="3" spans="2:12" ht="15" customHeight="1">
       <c r="B3" s="74" t="s">
         <v>0</v>
@@ -3008,7 +2943,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="2:12" ht="16.5" thickBot="1">
+    <row r="4" spans="2:12" ht="16" thickBot="1">
       <c r="B4" s="77"/>
       <c r="C4" s="78"/>
       <c r="D4" s="78"/>
@@ -3021,8 +2956,8 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="2:12" ht="16.5" thickBot="1"/>
-    <row r="6" spans="2:12" ht="16.5" thickBot="1">
+    <row r="5" spans="2:12" ht="16" thickBot="1"/>
+    <row r="6" spans="2:12" ht="16" thickBot="1">
       <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3025,7 @@
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -3108,24 +3043,24 @@
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="2:12" ht="16.5" thickBot="1">
+    <row r="14" spans="2:12" ht="16" thickBot="1">
       <c r="B14" s="59"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
     </row>
-    <row r="15" spans="2:12" ht="16.5" thickBot="1">
+    <row r="15" spans="2:12" ht="16" thickBot="1">
       <c r="B15" s="61" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="23.1" customHeight="1" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="23" customHeight="1" thickBot="1">
       <c r="B16" s="63" t="s">
         <v>18</v>
       </c>
@@ -3142,12 +3077,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="23.1" customHeight="1">
+    <row r="17" spans="2:6" ht="23" customHeight="1">
       <c r="B17" s="62">
         <v>1</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="62">
         <v>100</v>
@@ -3157,12 +3092,12 @@
       </c>
       <c r="F17" s="62"/>
     </row>
-    <row r="18" spans="2:6" ht="23.1" customHeight="1">
+    <row r="18" spans="2:6" ht="23" customHeight="1">
       <c r="B18" s="6">
         <v>2</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="6">
         <v>100</v>
@@ -3172,7 +3107,7 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="2:6" ht="23.1" customHeight="1">
+    <row r="19" spans="2:6" ht="23" customHeight="1">
       <c r="B19" s="6">
         <v>3</v>
       </c>
@@ -3187,7 +3122,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" ht="23.1" customHeight="1">
+    <row r="20" spans="2:6" ht="23" customHeight="1">
       <c r="B20" s="6">
         <v>4</v>
       </c>
@@ -3202,7 +3137,7 @@
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="2:6" ht="23.1" customHeight="1">
+    <row r="21" spans="2:6" ht="23" customHeight="1">
       <c r="B21" s="6">
         <v>5</v>
       </c>
@@ -3217,7 +3152,7 @@
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="2:6" ht="23.1" customHeight="1">
+    <row r="22" spans="2:6" ht="23" customHeight="1">
       <c r="B22" s="6">
         <v>6</v>
       </c>
@@ -3232,7 +3167,7 @@
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="2:6" ht="23.1" customHeight="1">
+    <row r="23" spans="2:6" ht="23" customHeight="1">
       <c r="B23" s="6">
         <v>7</v>
       </c>
@@ -3247,12 +3182,12 @@
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="2:6" ht="23.1" customHeight="1">
+    <row r="24" spans="2:6" ht="23" customHeight="1">
       <c r="B24" s="6">
         <v>8</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="6">
         <v>5</v>
@@ -3262,7 +3197,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="2:6" ht="23.1" customHeight="1">
+    <row r="25" spans="2:6" ht="23" customHeight="1">
       <c r="B25" s="6">
         <v>9</v>
       </c>
@@ -3277,7 +3212,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="2:6" ht="23.1" customHeight="1">
+    <row r="26" spans="2:6" ht="23" customHeight="1">
       <c r="B26" s="6">
         <v>10</v>
       </c>
@@ -3292,12 +3227,12 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="2:6" ht="23.1" customHeight="1">
+    <row r="27" spans="2:6" ht="23" customHeight="1">
       <c r="B27" s="6">
         <v>11</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="6">
         <v>100</v>
@@ -3307,7 +3242,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:6" ht="23.1" customHeight="1">
+    <row r="28" spans="2:6" ht="23" customHeight="1">
       <c r="B28" s="6">
         <v>12</v>
       </c>
@@ -3322,12 +3257,12 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6" ht="23.1" customHeight="1">
+    <row r="29" spans="2:6" ht="23" customHeight="1">
       <c r="B29" s="6">
         <v>13</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="6">
         <v>40</v>
@@ -3337,19 +3272,19 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6" ht="23.1" customHeight="1" thickBot="1">
+    <row r="30" spans="2:6" ht="23" customHeight="1" thickBot="1">
       <c r="B30" s="60"/>
       <c r="C30" s="60"/>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
     </row>
-    <row r="31" spans="2:6" ht="16.5" thickBot="1">
+    <row r="31" spans="2:6" ht="16" thickBot="1">
       <c r="B31" s="66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="16.5" thickBot="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="16" thickBot="1">
       <c r="B32" s="64" t="s">
         <v>18</v>
       </c>
@@ -3457,9 +3392,9 @@
     <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3474,14 +3409,14 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3492,7 +3427,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="71" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3500,31 +3435,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="82"/>
       <c r="B3" s="82"/>
       <c r="C3" s="73" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="82"/>
       <c r="B4" s="82"/>
       <c r="C4" s="73" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="82"/>
       <c r="B5" s="82"/>
       <c r="C5" s="73" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3532,24 +3467,24 @@
         <v>2</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="83"/>
       <c r="B7" s="83"/>
       <c r="C7" s="72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="83"/>
       <c r="B8" s="83"/>
       <c r="C8" s="72" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3560,21 +3495,21 @@
         <v>19</v>
       </c>
       <c r="C9" s="73" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="82"/>
       <c r="B10" s="82"/>
       <c r="C10" s="73" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="82"/>
       <c r="B11" s="82"/>
       <c r="C11" s="73" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3585,21 +3520,21 @@
         <v>20</v>
       </c>
       <c r="C12" s="72" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="83"/>
       <c r="B13" s="83"/>
       <c r="C13" s="72" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="83"/>
       <c r="B14" s="83"/>
       <c r="C14" s="72" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3610,28 +3545,28 @@
         <v>21</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="82"/>
       <c r="B16" s="82"/>
       <c r="C16" s="73" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="82"/>
       <c r="B17" s="82"/>
       <c r="C17" s="73" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="82"/>
       <c r="B18" s="82"/>
       <c r="C18" s="73" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3642,49 +3577,49 @@
         <v>22</v>
       </c>
       <c r="C19" s="72" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="83"/>
       <c r="B20" s="83"/>
       <c r="C20" s="72" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="83"/>
       <c r="B21" s="83"/>
       <c r="C21" s="72" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="83"/>
       <c r="B22" s="83"/>
       <c r="C22" s="72" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="83"/>
       <c r="B23" s="83"/>
       <c r="C23" s="72" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="83"/>
       <c r="B24" s="83"/>
       <c r="C24" s="72" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="83"/>
       <c r="B25" s="83"/>
       <c r="C25" s="72" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3695,35 +3630,35 @@
         <v>23</v>
       </c>
       <c r="C26" s="73" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="82"/>
       <c r="B27" s="82"/>
       <c r="C27" s="73" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="82"/>
       <c r="B28" s="82"/>
       <c r="C28" s="73" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="82"/>
       <c r="B29" s="82"/>
       <c r="C29" s="73" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="82"/>
       <c r="B30" s="82"/>
       <c r="C30" s="73" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3731,10 +3666,10 @@
         <v>8</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="72" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3745,21 +3680,21 @@
         <v>26</v>
       </c>
       <c r="C32" s="73" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="82"/>
       <c r="B33" s="82"/>
       <c r="C33" s="73" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="82"/>
       <c r="B34" s="82"/>
       <c r="C34" s="73" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3770,21 +3705,21 @@
         <v>24</v>
       </c>
       <c r="C35" s="72" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="83"/>
       <c r="B36" s="83"/>
       <c r="C36" s="72" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="83"/>
       <c r="B37" s="83"/>
       <c r="C37" s="72" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -3792,17 +3727,17 @@
         <v>11</v>
       </c>
       <c r="B38" s="82" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="73" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="82"/>
       <c r="B39" s="82"/>
       <c r="C39" s="73" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3813,14 +3748,14 @@
         <v>25</v>
       </c>
       <c r="C40" s="72" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="83"/>
       <c r="B41" s="83"/>
       <c r="C41" s="72" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3828,54 +3763,59 @@
         <v>13</v>
       </c>
       <c r="B42" s="82" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" s="73" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="82"/>
       <c r="B43" s="82"/>
       <c r="C43" s="73" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="82"/>
       <c r="B44" s="82"/>
       <c r="C44" s="73" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3883,19 +3823,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="13.375" customWidth="1"/>
+    <col min="1" max="2" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="87" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="88"/>
@@ -3930,7 +3870,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
@@ -3976,7 +3916,7 @@
       <c r="K5" s="24"/>
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:13" ht="16.5" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -3990,14 +3930,14 @@
       <c r="K6" s="24"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1">
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="D7" s="34"/>
       <c r="E7" s="33"/>
       <c r="F7" s="90" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="91"/>
       <c r="H7" s="91"/>
@@ -4006,7 +3946,7 @@
       <c r="K7" s="92"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1">
+    <row r="8" spans="1:13" ht="16" thickBot="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -4034,7 +3974,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" ht="31.5">
+    <row r="9" spans="1:13" ht="30">
       <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
@@ -4042,36 +3982,36 @@
         <v>15</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="48" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="52" t="s">
-        <v>78</v>
-      </c>
       <c r="I9" s="52" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="J9" s="52" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="K9" s="52" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="93" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
@@ -4084,7 +4024,7 @@
       <c r="J10" s="94"/>
       <c r="K10" s="94"/>
     </row>
-    <row r="11" spans="1:13" ht="31.5">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="35">
         <v>14</v>
       </c>
@@ -4095,7 +4035,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="37">
         <v>3</v>
@@ -4119,7 +4059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31.5">
+    <row r="12" spans="1:13" ht="30">
       <c r="A12" s="35">
         <v>14</v>
       </c>
@@ -4128,7 +4068,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="37">
         <v>1</v>
@@ -4152,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="63">
+    <row r="13" spans="1:13" ht="60">
       <c r="A13" s="35">
         <v>14</v>
       </c>
@@ -4161,7 +4101,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="37">
         <v>4</v>
@@ -4200,7 +4140,7 @@
       <c r="J14" s="94"/>
       <c r="K14" s="94"/>
     </row>
-    <row r="15" spans="1:13" ht="47.25">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="35">
         <v>15</v>
       </c>
@@ -4211,7 +4151,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="38">
         <v>3</v>
@@ -4235,7 +4175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="47.25">
+    <row r="16" spans="1:13" ht="45">
       <c r="A16" s="35">
         <v>15</v>
       </c>
@@ -4244,7 +4184,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="38">
         <v>4</v>
@@ -4268,7 +4208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="31.5">
+    <row r="17" spans="1:11" ht="30">
       <c r="A17" s="35">
         <v>15</v>
       </c>
@@ -4277,7 +4217,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="38">
         <v>3</v>
@@ -4301,7 +4241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="63">
+    <row r="18" spans="1:11" ht="60">
       <c r="A18" s="35">
         <v>15</v>
       </c>
@@ -4310,7 +4250,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="38">
         <v>10</v>
@@ -4349,7 +4289,7 @@
       <c r="J19" s="94"/>
       <c r="K19" s="94"/>
     </row>
-    <row r="20" spans="1:11" ht="47.25">
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="35">
         <v>16</v>
       </c>
@@ -4360,7 +4300,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="37">
         <v>20</v>
@@ -4384,7 +4324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="63">
+    <row r="21" spans="1:11" ht="60">
       <c r="A21" s="35">
         <v>16</v>
       </c>
@@ -4393,7 +4333,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="37">
         <v>5</v>
@@ -4417,7 +4357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="63">
+    <row r="22" spans="1:11" ht="60">
       <c r="A22" s="35">
         <v>16</v>
       </c>
@@ -4426,7 +4366,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="37">
         <v>15</v>
@@ -4465,7 +4405,7 @@
       <c r="J23" s="94"/>
       <c r="K23" s="94"/>
     </row>
-    <row r="24" spans="1:11" ht="47.25">
+    <row r="24" spans="1:11" ht="45">
       <c r="A24" s="35">
         <v>17</v>
       </c>
@@ -4476,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="40">
         <v>1</v>
@@ -4500,7 +4440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="31.5">
+    <row r="25" spans="1:11" ht="30">
       <c r="A25" s="35">
         <v>17</v>
       </c>
@@ -4509,7 +4449,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="40">
         <v>1</v>
@@ -4533,7 +4473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="63">
+    <row r="26" spans="1:11" ht="60">
       <c r="A26" s="35">
         <v>17</v>
       </c>
@@ -4542,7 +4482,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="40">
         <v>1</v>
@@ -4581,7 +4521,7 @@
       <c r="J27" s="94"/>
       <c r="K27" s="94"/>
     </row>
-    <row r="28" spans="1:11" ht="31.5">
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="35">
         <v>18</v>
       </c>
@@ -4592,7 +4532,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E28" s="37">
         <v>5</v>
@@ -4616,7 +4556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="31.5">
+    <row r="29" spans="1:11" ht="30">
       <c r="A29" s="35">
         <v>18</v>
       </c>
@@ -4625,7 +4565,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="37">
         <v>5</v>
@@ -4649,7 +4589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="47.25">
+    <row r="30" spans="1:11" ht="45">
       <c r="A30" s="35">
         <v>18</v>
       </c>
@@ -4658,7 +4598,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="37">
         <v>10</v>
@@ -4682,7 +4622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="47.25">
+    <row r="31" spans="1:11" ht="45">
       <c r="A31" s="35">
         <v>18</v>
       </c>
@@ -4691,7 +4631,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E31" s="40">
         <v>5</v>
@@ -4715,7 +4655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="31.5">
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="35">
         <v>18</v>
       </c>
@@ -4724,7 +4664,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" s="40">
         <v>15</v>
@@ -4748,12 +4688,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="31.5">
+    <row r="33" spans="1:13" ht="30">
       <c r="A33" s="33"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
       <c r="D33" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="26">
         <f>SUM(E11:E32)</f>
@@ -4785,12 +4725,12 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="47.25">
+    <row r="34" spans="1:13" ht="45">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
       <c r="D34" s="57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34" s="26">
         <f>SUM(E11:E32)</f>

</xml_diff>

<commit_message>
WS ListeConseiller et ListeCompte
WS ListeConseiller et ListeCompte(tout les comptes) et ListeComptesbyId(pour un client)
</commit_message>
<xml_diff>
--- a/ProxiV4 - Product backlog.xlsx
+++ b/ProxiV4 - Product backlog.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminl\Desktop\Rob\depot git\ProxiBanqueV4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25700" yWindow="0" windowWidth="29300" windowHeight="17180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="29295" windowHeight="17175" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
     <sheet name="tâches User Stories" sheetId="3" r:id="rId2"/>
     <sheet name="Sprint 0" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="126">
   <si>
     <t>ProxiBanqueV4 - Product Balcklog</t>
   </si>
@@ -409,7 +415,7 @@
     <numFmt numFmtId="164" formatCode="ddd\ dd/mm"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -529,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -941,6 +947,26 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -955,7 +981,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1172,6 +1198,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1252,19 +1287,80 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="57"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="57"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1490,7 +1586,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1536,6 +1632,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1580,25 +1696,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1610,25 +1726,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>111.0</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1672,25 +1788,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1702,25 +1818,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>111.0</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,11 +1853,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2096667832"/>
-        <c:axId val="-2131276376"/>
+        <c:axId val="141008976"/>
+        <c:axId val="141009536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2096667832"/>
+        <c:axId val="141008976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1782,6 +1898,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1817,10 +1953,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131276376"/>
+        <c:crossAx val="141009536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1828,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131276376"/>
+        <c:axId val="141009536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1883,6 +2019,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1912,11 +2068,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096667832"/>
-        <c:crossesAt val="1.0"/>
+        <c:crossAx val="141008976"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1955,7 +2111,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1985,7 +2141,576 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Burn Down Chart Sprint 0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Points d'effort optimaux</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$34:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Points d'effort réalisés</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 0'!$E$33:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="221455648"/>
+        <c:axId val="221461808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="221455648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221461808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="221461808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Points d'effort</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="221455648"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1997,6 +2722,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2539,6 +3304,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2574,15 +3842,52 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B16:F29" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B16:F29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="B16:F29"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="User Story ID" dataDxfId="6"/>
-    <tableColumn id="2" name="User Story" dataDxfId="5"/>
-    <tableColumn id="3" name="Priorité" dataDxfId="4"/>
-    <tableColumn id="4" name="Estimation (complexité)" dataDxfId="3"/>
-    <tableColumn id="5" name="Sprint n°" dataDxfId="2"/>
+    <tableColumn id="1" name="User Story ID" dataDxfId="10"/>
+    <tableColumn id="2" name="User Story" dataDxfId="9"/>
+    <tableColumn id="3" name="Priorité" dataDxfId="8"/>
+    <tableColumn id="4" name="Estimation (complexité)" dataDxfId="7"/>
+    <tableColumn id="5" name="Sprint n°" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2913,29 +4218,29 @@
   <dimension ref="B2:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="62.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="16" thickBot="1"/>
+    <row r="2" spans="2:12" ht="16.5" thickBot="1"/>
     <row r="3" spans="2:12" ht="15" customHeight="1">
-      <c r="B3" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
+      <c r="B3" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="79"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -2943,12 +4248,12 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="2:12" ht="16" thickBot="1">
-      <c r="B4" s="77"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
+    <row r="4" spans="2:12" ht="16.5" thickBot="1">
+      <c r="B4" s="80"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -2956,8 +4261,8 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="2:12" ht="16" thickBot="1"/>
-    <row r="6" spans="2:12" ht="16" thickBot="1">
+    <row r="5" spans="2:12" ht="16.5" thickBot="1"/>
+    <row r="6" spans="2:12" ht="16.5" thickBot="1">
       <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
@@ -2986,7 +4291,7 @@
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="83" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -3000,7 +4305,7 @@
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="81"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -3012,7 +4317,7 @@
       </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="81"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
@@ -3050,17 +4355,17 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="2:12" ht="16" thickBot="1">
+    <row r="14" spans="2:12" ht="16.5" thickBot="1">
       <c r="B14" s="59"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
     </row>
-    <row r="15" spans="2:12" ht="16" thickBot="1">
+    <row r="15" spans="2:12" ht="16.5" thickBot="1">
       <c r="B15" s="61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="23" customHeight="1" thickBot="1">
+    <row r="16" spans="2:12" ht="23.1" customHeight="1" thickBot="1">
       <c r="B16" s="63" t="s">
         <v>18</v>
       </c>
@@ -3077,7 +4382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="23" customHeight="1">
+    <row r="17" spans="2:6" ht="23.1" customHeight="1">
       <c r="B17" s="62">
         <v>1</v>
       </c>
@@ -3092,7 +4397,7 @@
       </c>
       <c r="F17" s="62"/>
     </row>
-    <row r="18" spans="2:6" ht="23" customHeight="1">
+    <row r="18" spans="2:6" ht="23.1" customHeight="1">
       <c r="B18" s="6">
         <v>2</v>
       </c>
@@ -3107,7 +4412,7 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="2:6" ht="23" customHeight="1">
+    <row r="19" spans="2:6" ht="23.1" customHeight="1">
       <c r="B19" s="6">
         <v>3</v>
       </c>
@@ -3122,7 +4427,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" ht="23" customHeight="1">
+    <row r="20" spans="2:6" ht="23.1" customHeight="1">
       <c r="B20" s="6">
         <v>4</v>
       </c>
@@ -3137,7 +4442,7 @@
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="2:6" ht="23" customHeight="1">
+    <row r="21" spans="2:6" ht="23.1" customHeight="1">
       <c r="B21" s="6">
         <v>5</v>
       </c>
@@ -3152,7 +4457,7 @@
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="2:6" ht="23" customHeight="1">
+    <row r="22" spans="2:6" ht="23.1" customHeight="1">
       <c r="B22" s="6">
         <v>6</v>
       </c>
@@ -3167,7 +4472,7 @@
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="2:6" ht="23" customHeight="1">
+    <row r="23" spans="2:6" ht="23.1" customHeight="1">
       <c r="B23" s="6">
         <v>7</v>
       </c>
@@ -3182,7 +4487,7 @@
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="2:6" ht="23" customHeight="1">
+    <row r="24" spans="2:6" ht="23.1" customHeight="1">
       <c r="B24" s="6">
         <v>8</v>
       </c>
@@ -3197,7 +4502,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="2:6" ht="23" customHeight="1">
+    <row r="25" spans="2:6" ht="23.1" customHeight="1">
       <c r="B25" s="6">
         <v>9</v>
       </c>
@@ -3212,7 +4517,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="2:6" ht="23" customHeight="1">
+    <row r="26" spans="2:6" ht="23.1" customHeight="1">
       <c r="B26" s="6">
         <v>10</v>
       </c>
@@ -3227,7 +4532,7 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="2:6" ht="23" customHeight="1">
+    <row r="27" spans="2:6" ht="23.1" customHeight="1">
       <c r="B27" s="6">
         <v>11</v>
       </c>
@@ -3242,7 +4547,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:6" ht="23" customHeight="1">
+    <row r="28" spans="2:6" ht="23.1" customHeight="1">
       <c r="B28" s="6">
         <v>12</v>
       </c>
@@ -3257,7 +4562,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6" ht="23" customHeight="1">
+    <row r="29" spans="2:6" ht="23.1" customHeight="1">
       <c r="B29" s="6">
         <v>13</v>
       </c>
@@ -3272,19 +4577,19 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6" ht="23" customHeight="1" thickBot="1">
+    <row r="30" spans="2:6" ht="23.1" customHeight="1" thickBot="1">
       <c r="B30" s="60"/>
       <c r="C30" s="60"/>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
     </row>
-    <row r="31" spans="2:6" ht="16" thickBot="1">
+    <row r="31" spans="2:6" ht="16.5" thickBot="1">
       <c r="B31" s="66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="16" thickBot="1">
+    <row r="32" spans="2:6" ht="16.5" thickBot="1">
       <c r="B32" s="64" t="s">
         <v>18</v>
       </c>
@@ -3408,15 +4713,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3431,10 +4736,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="82">
+      <c r="A2" s="85">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="85" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="73" t="s">
@@ -3442,31 +4747,31 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="82"/>
-      <c r="B3" s="82"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="73" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="82"/>
-      <c r="B4" s="82"/>
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="73" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="73" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="83">
+      <c r="A6" s="86">
         <v>2</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="86" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="72" t="s">
@@ -3474,24 +4779,24 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="72" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="72" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="82">
+      <c r="A9" s="85">
         <v>3</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="85" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="73" t="s">
@@ -3499,24 +4804,24 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="82"/>
-      <c r="B10" s="82"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="73" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="82"/>
-      <c r="B11" s="82"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="73" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="83">
+      <c r="A12" s="86">
         <v>4</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="86" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="72" t="s">
@@ -3524,24 +4829,24 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="83"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="72" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="83"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="72" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="82">
+      <c r="A15" s="85">
         <v>5</v>
       </c>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="85" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="73" t="s">
@@ -3549,31 +4854,31 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="82"/>
-      <c r="B16" s="82"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="85"/>
       <c r="C16" s="73" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="82"/>
-      <c r="B17" s="82"/>
+      <c r="A17" s="85"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="73" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="85"/>
       <c r="C18" s="73" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="83">
+      <c r="A19" s="86">
         <v>6</v>
       </c>
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="86" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="72" t="s">
@@ -3581,52 +4886,52 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83"/>
+      <c r="A20" s="86"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="72" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="83"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="72" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="83"/>
-      <c r="B22" s="83"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="72" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
+      <c r="A23" s="86"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="72" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="72" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="83"/>
-      <c r="B25" s="83"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="72" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="82">
+      <c r="A26" s="85">
         <v>7</v>
       </c>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="85" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="73" t="s">
@@ -3634,29 +4939,29 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="82"/>
-      <c r="B27" s="82"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="85"/>
       <c r="C27" s="73" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="82"/>
-      <c r="B28" s="82"/>
+      <c r="A28" s="85"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="73" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="82"/>
-      <c r="B29" s="82"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="73" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="82"/>
-      <c r="B30" s="82"/>
+      <c r="A30" s="85"/>
+      <c r="B30" s="85"/>
       <c r="C30" s="73" t="s">
         <v>107</v>
       </c>
@@ -3673,10 +4978,10 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="82">
+      <c r="A32" s="85">
         <v>9</v>
       </c>
-      <c r="B32" s="82" t="s">
+      <c r="B32" s="85" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="73" t="s">
@@ -3684,24 +4989,24 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="82"/>
-      <c r="B33" s="82"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="73" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="82"/>
-      <c r="B34" s="82"/>
+      <c r="A34" s="85"/>
+      <c r="B34" s="85"/>
       <c r="C34" s="73" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="83">
+      <c r="A35" s="86">
         <v>10</v>
       </c>
-      <c r="B35" s="83" t="s">
+      <c r="B35" s="86" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="72" t="s">
@@ -3709,24 +5014,24 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
+      <c r="A36" s="86"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="72" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="86"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="72" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="82">
+      <c r="A38" s="85">
         <v>11</v>
       </c>
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="85" t="s">
         <v>70</v>
       </c>
       <c r="C38" s="73" t="s">
@@ -3734,17 +5039,17 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="82"/>
-      <c r="B39" s="82"/>
+      <c r="A39" s="85"/>
+      <c r="B39" s="85"/>
       <c r="C39" s="73" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="83">
+      <c r="A40" s="86">
         <v>12</v>
       </c>
-      <c r="B40" s="83" t="s">
+      <c r="B40" s="86" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="72" t="s">
@@ -3752,17 +5057,17 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="83"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="86"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="72" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="82">
+      <c r="A42" s="85">
         <v>13</v>
       </c>
-      <c r="B42" s="82" t="s">
+      <c r="B42" s="85" t="s">
         <v>75</v>
       </c>
       <c r="C42" s="73" t="s">
@@ -3770,45 +5075,45 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="82"/>
-      <c r="B43" s="82"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="85"/>
       <c r="C43" s="73" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="82"/>
-      <c r="B44" s="82"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="85"/>
       <c r="C44" s="73" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="B19:B25"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3824,29 +5129,29 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="M13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="2" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="22"/>
@@ -3916,7 +5221,7 @@
       <c r="K5" s="24"/>
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:13" ht="16" thickBot="1">
+    <row r="6" spans="1:13" ht="16.5" thickBot="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -3930,23 +5235,23 @@
       <c r="K6" s="24"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="16" thickBot="1">
+    <row r="7" spans="1:13" ht="16.5" thickBot="1">
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="D7" s="34"/>
       <c r="E7" s="33"/>
-      <c r="F7" s="90" t="s">
+      <c r="F7" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="92"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1">
+    <row r="8" spans="1:13" ht="16.5" thickBot="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -3974,7 +5279,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" ht="30">
+    <row r="9" spans="1:13" ht="31.5">
       <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
@@ -4010,25 +5315,25 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-    </row>
-    <row r="11" spans="1:13" ht="45">
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.5">
       <c r="A11" s="35">
         <v>14</v>
       </c>
-      <c r="B11" s="84">
+      <c r="B11" s="87">
         <v>8</v>
       </c>
       <c r="C11" s="36">
@@ -4059,11 +5364,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30">
+    <row r="12" spans="1:13" ht="31.5">
       <c r="A12" s="35">
         <v>14</v>
       </c>
-      <c r="B12" s="85"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="36">
         <v>2</v>
       </c>
@@ -4092,11 +5397,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60">
+    <row r="13" spans="1:13" ht="63">
       <c r="A13" s="35">
         <v>14</v>
       </c>
-      <c r="B13" s="86"/>
+      <c r="B13" s="89"/>
       <c r="C13" s="36">
         <v>3</v>
       </c>
@@ -4126,25 +5431,25 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-    </row>
-    <row r="15" spans="1:13" ht="45">
+      <c r="B14" s="97"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+    </row>
+    <row r="15" spans="1:13" ht="47.25">
       <c r="A15" s="35">
         <v>15</v>
       </c>
-      <c r="B15" s="84">
+      <c r="B15" s="87">
         <v>20</v>
       </c>
       <c r="C15" s="36">
@@ -4175,11 +5480,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45">
+    <row r="16" spans="1:13" ht="47.25">
       <c r="A16" s="35">
         <v>15</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="36">
         <v>2</v>
       </c>
@@ -4208,11 +5513,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30">
+    <row r="17" spans="1:11" ht="31.5">
       <c r="A17" s="35">
         <v>15</v>
       </c>
-      <c r="B17" s="85"/>
+      <c r="B17" s="88"/>
       <c r="C17" s="36">
         <v>3</v>
       </c>
@@ -4241,11 +5546,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="60">
+    <row r="18" spans="1:11" ht="63">
       <c r="A18" s="35">
         <v>15</v>
       </c>
-      <c r="B18" s="86"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="36">
         <v>4</v>
       </c>
@@ -4275,25 +5580,25 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="94"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="94"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="94"/>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+    </row>
+    <row r="20" spans="1:11" ht="47.25">
       <c r="A20" s="35">
         <v>16</v>
       </c>
-      <c r="B20" s="84">
+      <c r="B20" s="87">
         <v>3</v>
       </c>
       <c r="C20" s="36">
@@ -4324,11 +5629,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="60">
+    <row r="21" spans="1:11" ht="63">
       <c r="A21" s="35">
         <v>16</v>
       </c>
-      <c r="B21" s="85"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="36">
         <v>2</v>
       </c>
@@ -4357,11 +5662,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="63">
       <c r="A22" s="35">
         <v>16</v>
       </c>
-      <c r="B22" s="86"/>
+      <c r="B22" s="89"/>
       <c r="C22" s="36">
         <v>3</v>
       </c>
@@ -4391,25 +5696,25 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="94"/>
-    </row>
-    <row r="24" spans="1:11" ht="45">
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+    </row>
+    <row r="24" spans="1:11" ht="47.25">
       <c r="A24" s="35">
         <v>17</v>
       </c>
-      <c r="B24" s="96">
+      <c r="B24" s="99">
         <v>40</v>
       </c>
       <c r="C24" s="35">
@@ -4440,11 +5745,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30">
+    <row r="25" spans="1:11" ht="31.5">
       <c r="A25" s="35">
         <v>17</v>
       </c>
-      <c r="B25" s="97"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="35">
         <v>2</v>
       </c>
@@ -4473,11 +5778,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60">
+    <row r="26" spans="1:11" ht="63">
       <c r="A26" s="35">
         <v>17</v>
       </c>
-      <c r="B26" s="98"/>
+      <c r="B26" s="101"/>
       <c r="C26" s="35">
         <v>3</v>
       </c>
@@ -4507,25 +5812,25 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="94"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="94"/>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+    </row>
+    <row r="28" spans="1:11" ht="31.5">
       <c r="A28" s="35">
         <v>18</v>
       </c>
-      <c r="B28" s="84">
+      <c r="B28" s="87">
         <v>40</v>
       </c>
       <c r="C28" s="36">
@@ -4556,11 +5861,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30">
+    <row r="29" spans="1:11" ht="31.5">
       <c r="A29" s="35">
         <v>18</v>
       </c>
-      <c r="B29" s="85"/>
+      <c r="B29" s="88"/>
       <c r="C29" s="36">
         <v>2</v>
       </c>
@@ -4589,11 +5894,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45">
+    <row r="30" spans="1:11" ht="47.25">
       <c r="A30" s="35">
         <v>18</v>
       </c>
-      <c r="B30" s="85"/>
+      <c r="B30" s="88"/>
       <c r="C30" s="36">
         <v>3</v>
       </c>
@@ -4622,11 +5927,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45">
+    <row r="31" spans="1:11" ht="47.25">
       <c r="A31" s="35">
         <v>18</v>
       </c>
-      <c r="B31" s="85"/>
+      <c r="B31" s="88"/>
       <c r="C31" s="36">
         <v>4</v>
       </c>
@@ -4655,11 +5960,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30">
+    <row r="32" spans="1:11" ht="31.5">
       <c r="A32" s="35">
         <v>18</v>
       </c>
-      <c r="B32" s="86"/>
+      <c r="B32" s="89"/>
       <c r="C32" s="36">
         <v>5</v>
       </c>
@@ -4688,7 +5993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30">
+    <row r="33" spans="1:13" ht="31.5">
       <c r="A33" s="33"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
@@ -4725,7 +6030,7 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="45">
+    <row r="34" spans="1:13" ht="47.25">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -4791,10 +6096,10 @@
     <mergeCell ref="B24:B26"/>
   </mergeCells>
   <conditionalFormatting sqref="F33:K33">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>F34</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>F34</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4807,4 +6112,980 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="2" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="62.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="M2" s="21"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="M3" s="21"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="28">
+        <v>43108</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="M5" s="21"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="M6" s="21"/>
+    </row>
+    <row r="7" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="95"/>
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="74">
+        <v>0</v>
+      </c>
+      <c r="F8" s="75">
+        <v>1</v>
+      </c>
+      <c r="G8" s="75">
+        <v>2</v>
+      </c>
+      <c r="H8" s="75">
+        <v>3</v>
+      </c>
+      <c r="I8" s="75">
+        <v>4</v>
+      </c>
+      <c r="J8" s="75">
+        <v>5</v>
+      </c>
+      <c r="K8" s="76">
+        <v>6</v>
+      </c>
+      <c r="M8" s="21"/>
+    </row>
+    <row r="9" spans="1:13" ht="31.5">
+      <c r="A9" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="K9" s="52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="104">
+        <v>1</v>
+      </c>
+      <c r="B11" s="103">
+        <v>20</v>
+      </c>
+      <c r="C11" s="107">
+        <v>1</v>
+      </c>
+      <c r="D11" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="37">
+        <v>5</v>
+      </c>
+      <c r="F11" s="35">
+        <v>5</v>
+      </c>
+      <c r="G11" s="35">
+        <v>5</v>
+      </c>
+      <c r="H11" s="35">
+        <v>5</v>
+      </c>
+      <c r="I11" s="35">
+        <v>5</v>
+      </c>
+      <c r="J11" s="35">
+        <v>5</v>
+      </c>
+      <c r="K11" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="105"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="107">
+        <v>2</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="37">
+        <v>8</v>
+      </c>
+      <c r="F12" s="35">
+        <v>0</v>
+      </c>
+      <c r="G12" s="35">
+        <v>4</v>
+      </c>
+      <c r="H12" s="35">
+        <v>4</v>
+      </c>
+      <c r="I12" s="35">
+        <v>8</v>
+      </c>
+      <c r="J12" s="35">
+        <v>8</v>
+      </c>
+      <c r="K12" s="35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A13" s="105"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="107">
+        <v>3</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="38">
+        <v>4</v>
+      </c>
+      <c r="F13" s="35">
+        <v>0</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="35">
+        <v>0</v>
+      </c>
+      <c r="I13" s="35">
+        <v>4</v>
+      </c>
+      <c r="J13" s="35">
+        <v>4</v>
+      </c>
+      <c r="K13" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A14" s="106"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="102">
+        <v>4</v>
+      </c>
+      <c r="D14" s="108" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="110">
+        <v>3</v>
+      </c>
+      <c r="F14" s="107">
+        <v>0</v>
+      </c>
+      <c r="G14" s="35">
+        <v>0</v>
+      </c>
+      <c r="H14" s="35">
+        <v>0</v>
+      </c>
+      <c r="I14" s="35">
+        <v>0</v>
+      </c>
+      <c r="J14" s="35">
+        <v>3</v>
+      </c>
+      <c r="K14" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="97"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="99">
+        <v>2</v>
+      </c>
+      <c r="B16" s="87">
+        <v>8</v>
+      </c>
+      <c r="C16" s="36">
+        <v>1</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="38">
+        <v>3</v>
+      </c>
+      <c r="F16" s="39">
+        <v>3</v>
+      </c>
+      <c r="G16" s="39">
+        <v>3</v>
+      </c>
+      <c r="H16" s="39">
+        <v>3</v>
+      </c>
+      <c r="I16" s="39">
+        <v>3</v>
+      </c>
+      <c r="J16" s="39">
+        <v>3</v>
+      </c>
+      <c r="K16" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="100"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="36">
+        <v>2</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="38">
+        <v>4</v>
+      </c>
+      <c r="F17" s="39">
+        <v>0</v>
+      </c>
+      <c r="G17" s="39">
+        <v>4</v>
+      </c>
+      <c r="H17" s="39">
+        <v>4</v>
+      </c>
+      <c r="I17" s="39">
+        <v>4</v>
+      </c>
+      <c r="J17" s="39">
+        <v>4</v>
+      </c>
+      <c r="K17" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="100"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="36">
+        <v>3</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="38">
+        <v>3</v>
+      </c>
+      <c r="F18" s="39">
+        <v>0</v>
+      </c>
+      <c r="G18" s="39">
+        <v>0</v>
+      </c>
+      <c r="H18" s="39">
+        <v>0</v>
+      </c>
+      <c r="I18" s="39">
+        <v>3</v>
+      </c>
+      <c r="J18" s="39">
+        <v>3</v>
+      </c>
+      <c r="K18" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+    </row>
+    <row r="20" spans="1:11" ht="47.25">
+      <c r="A20" s="35">
+        <v>16</v>
+      </c>
+      <c r="B20" s="87">
+        <v>3</v>
+      </c>
+      <c r="C20" s="36">
+        <v>1</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="37">
+        <v>20</v>
+      </c>
+      <c r="F20" s="35">
+        <v>10</v>
+      </c>
+      <c r="G20" s="35">
+        <v>15</v>
+      </c>
+      <c r="H20" s="35">
+        <v>20</v>
+      </c>
+      <c r="I20" s="35">
+        <v>20</v>
+      </c>
+      <c r="J20" s="35">
+        <v>20</v>
+      </c>
+      <c r="K20" s="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="63">
+      <c r="A21" s="35">
+        <v>16</v>
+      </c>
+      <c r="B21" s="88"/>
+      <c r="C21" s="36">
+        <v>2</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="37">
+        <v>5</v>
+      </c>
+      <c r="F21" s="35">
+        <v>0</v>
+      </c>
+      <c r="G21" s="35">
+        <v>0</v>
+      </c>
+      <c r="H21" s="35">
+        <v>5</v>
+      </c>
+      <c r="I21" s="35">
+        <v>5</v>
+      </c>
+      <c r="J21" s="35">
+        <v>5</v>
+      </c>
+      <c r="K21" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="63">
+      <c r="A22" s="35">
+        <v>16</v>
+      </c>
+      <c r="B22" s="89"/>
+      <c r="C22" s="36">
+        <v>3</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="37">
+        <v>15</v>
+      </c>
+      <c r="F22" s="35">
+        <v>0</v>
+      </c>
+      <c r="G22" s="35">
+        <v>0</v>
+      </c>
+      <c r="H22" s="35">
+        <v>0</v>
+      </c>
+      <c r="I22" s="35">
+        <v>5</v>
+      </c>
+      <c r="J22" s="35">
+        <v>10</v>
+      </c>
+      <c r="K22" s="35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+    </row>
+    <row r="24" spans="1:11" ht="47.25">
+      <c r="A24" s="35">
+        <v>17</v>
+      </c>
+      <c r="B24" s="99">
+        <v>40</v>
+      </c>
+      <c r="C24" s="35">
+        <v>1</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="40">
+        <v>1</v>
+      </c>
+      <c r="F24" s="39">
+        <v>0</v>
+      </c>
+      <c r="G24" s="39">
+        <v>0</v>
+      </c>
+      <c r="H24" s="39">
+        <v>0</v>
+      </c>
+      <c r="I24" s="39">
+        <v>1</v>
+      </c>
+      <c r="J24" s="39">
+        <v>1</v>
+      </c>
+      <c r="K24" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="31.5">
+      <c r="A25" s="35">
+        <v>17</v>
+      </c>
+      <c r="B25" s="100"/>
+      <c r="C25" s="35">
+        <v>2</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="40">
+        <v>1</v>
+      </c>
+      <c r="F25" s="39">
+        <v>0</v>
+      </c>
+      <c r="G25" s="39">
+        <v>0</v>
+      </c>
+      <c r="H25" s="39">
+        <v>0</v>
+      </c>
+      <c r="I25" s="39">
+        <v>0</v>
+      </c>
+      <c r="J25" s="39">
+        <v>1</v>
+      </c>
+      <c r="K25" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="63">
+      <c r="A26" s="35">
+        <v>17</v>
+      </c>
+      <c r="B26" s="101"/>
+      <c r="C26" s="35">
+        <v>3</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="40">
+        <v>1</v>
+      </c>
+      <c r="F26" s="39">
+        <v>0</v>
+      </c>
+      <c r="G26" s="39">
+        <v>0</v>
+      </c>
+      <c r="H26" s="39">
+        <v>0</v>
+      </c>
+      <c r="I26" s="39">
+        <v>0</v>
+      </c>
+      <c r="J26" s="39">
+        <v>0</v>
+      </c>
+      <c r="K26" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="98" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+    </row>
+    <row r="28" spans="1:11" ht="31.5">
+      <c r="A28" s="35">
+        <v>18</v>
+      </c>
+      <c r="B28" s="87">
+        <v>40</v>
+      </c>
+      <c r="C28" s="36">
+        <v>1</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="37">
+        <v>5</v>
+      </c>
+      <c r="F28" s="39">
+        <v>5</v>
+      </c>
+      <c r="G28" s="39">
+        <v>5</v>
+      </c>
+      <c r="H28" s="39">
+        <v>5</v>
+      </c>
+      <c r="I28" s="39">
+        <v>5</v>
+      </c>
+      <c r="J28" s="39">
+        <v>5</v>
+      </c>
+      <c r="K28" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="31.5">
+      <c r="A29" s="35">
+        <v>18</v>
+      </c>
+      <c r="B29" s="88"/>
+      <c r="C29" s="36">
+        <v>2</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="37">
+        <v>5</v>
+      </c>
+      <c r="F29" s="39">
+        <v>0</v>
+      </c>
+      <c r="G29" s="39">
+        <v>5</v>
+      </c>
+      <c r="H29" s="39">
+        <v>5</v>
+      </c>
+      <c r="I29" s="39">
+        <v>5</v>
+      </c>
+      <c r="J29" s="39">
+        <v>5</v>
+      </c>
+      <c r="K29" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="47.25">
+      <c r="A30" s="35">
+        <v>18</v>
+      </c>
+      <c r="B30" s="88"/>
+      <c r="C30" s="36">
+        <v>3</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="37">
+        <v>10</v>
+      </c>
+      <c r="F30" s="39">
+        <v>0</v>
+      </c>
+      <c r="G30" s="39">
+        <v>0</v>
+      </c>
+      <c r="H30" s="39">
+        <v>10</v>
+      </c>
+      <c r="I30" s="39">
+        <v>10</v>
+      </c>
+      <c r="J30" s="39">
+        <v>10</v>
+      </c>
+      <c r="K30" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="47.25">
+      <c r="A31" s="35">
+        <v>18</v>
+      </c>
+      <c r="B31" s="88"/>
+      <c r="C31" s="36">
+        <v>4</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="40">
+        <v>5</v>
+      </c>
+      <c r="F31" s="39">
+        <v>0</v>
+      </c>
+      <c r="G31" s="39">
+        <v>0</v>
+      </c>
+      <c r="H31" s="39">
+        <v>5</v>
+      </c>
+      <c r="I31" s="39">
+        <v>5</v>
+      </c>
+      <c r="J31" s="39">
+        <v>5</v>
+      </c>
+      <c r="K31" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="31.5">
+      <c r="A32" s="35">
+        <v>18</v>
+      </c>
+      <c r="B32" s="89"/>
+      <c r="C32" s="36">
+        <v>5</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="40">
+        <v>15</v>
+      </c>
+      <c r="F32" s="39">
+        <v>0</v>
+      </c>
+      <c r="G32" s="39">
+        <v>0</v>
+      </c>
+      <c r="H32" s="39">
+        <v>0</v>
+      </c>
+      <c r="I32" s="39">
+        <v>0</v>
+      </c>
+      <c r="J32" s="39">
+        <v>15</v>
+      </c>
+      <c r="K32" s="39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="31.5">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="26">
+        <f>SUM(E11:E32)</f>
+        <v>113</v>
+      </c>
+      <c r="F33" s="41">
+        <f>$E33-SUM(F11:F32)</f>
+        <v>90</v>
+      </c>
+      <c r="G33" s="41">
+        <f>$E33-SUM(G11:G32)</f>
+        <v>72</v>
+      </c>
+      <c r="H33" s="41">
+        <f>$E33-SUM(H11:H32)</f>
+        <v>47</v>
+      </c>
+      <c r="I33" s="41">
+        <f>$E33-SUM(I11:I32)</f>
+        <v>30</v>
+      </c>
+      <c r="J33" s="41">
+        <f>$E33-SUM(J11:J32)</f>
+        <v>6</v>
+      </c>
+      <c r="K33" s="41">
+        <f>$E33-SUM(K11:K32)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="21"/>
+    </row>
+    <row r="34" spans="1:13" ht="47.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="26">
+        <f>SUM(E11:E32)</f>
+        <v>113</v>
+      </c>
+      <c r="F34" s="42">
+        <f>-(E34/K8)*F8+E34</f>
+        <v>94.166666666666671</v>
+      </c>
+      <c r="G34" s="42">
+        <f>-($E34/$K8)*G8+$E34</f>
+        <v>75.333333333333343</v>
+      </c>
+      <c r="H34" s="42">
+        <f>-($E34/$K8)*H8+$E34</f>
+        <v>56.5</v>
+      </c>
+      <c r="I34" s="42">
+        <f>-($E34/$K8)*I8+$E34</f>
+        <v>37.666666666666671</v>
+      </c>
+      <c r="J34" s="42">
+        <f>-($E34/$K8)*J8+$E34</f>
+        <v>18.833333333333343</v>
+      </c>
+      <c r="K34" s="42">
+        <f>-($E34/$K8)*K8+$E34</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="21"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="45"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A19:K19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:K23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A16:A18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F33:K33">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+      <formula>F34</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
+      <formula>F34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit lean et PB
</commit_message>
<xml_diff>
--- a/ProxiV4 - Product backlog.xlsx
+++ b/ProxiV4 - Product backlog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminl\Desktop\Rob\depot git\ProxiBanqueV4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14535" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sprint 0" sheetId="2" r:id="rId3"/>
     <sheet name="Sprint 1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="144">
   <si>
     <t>ProxiBanqueV4 - Product Balcklog</t>
   </si>
@@ -270,9 +275,6 @@
     <t>3) verifier en base de données si il existe</t>
   </si>
   <si>
-    <t>4) coder une alerte si connexion incorrecte ou page d'accueil.</t>
-  </si>
-  <si>
     <t>1) coder page de déconnection</t>
   </si>
   <si>
@@ -282,24 +284,12 @@
     <t>3) renvoyer sur la page de connection</t>
   </si>
   <si>
-    <t>1) après login, recuperer la liste de clients du conseiller (webservice)</t>
-  </si>
-  <si>
-    <t>2) en fonction du conseiller logé, afficher la liste de clients associés</t>
-  </si>
-  <si>
-    <t>3) possibilités d'actions pour chaque clients</t>
-  </si>
-  <si>
     <t>1) recupérer l'id du client et transmettre au WS</t>
   </si>
   <si>
     <t>2) recupérer ses comptes (webservice)</t>
   </si>
   <si>
-    <t>3) afficher ses comptes sur une page</t>
-  </si>
-  <si>
     <t>1) Récupérer l'id du client sélectionné et le transmettre au WS</t>
   </si>
   <si>
@@ -384,9 +374,6 @@
     <t>En tant que conseiller je veux recevoir une alerte des clients à découvert</t>
   </si>
   <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
     <t>10h00</t>
   </si>
   <si>
@@ -421,6 +408,57 @@
   </si>
   <si>
     <t>6)Afficher un message de succès/d'échec du virement</t>
+  </si>
+  <si>
+    <t>Sprint 1 Back Office</t>
+  </si>
+  <si>
+    <t>4) renvoyer la reponse de la requette</t>
+  </si>
+  <si>
+    <t>5) coder une alerte si connexion incorrecte ou page d'accueil.</t>
+  </si>
+  <si>
+    <t>2) webservice renvoit la liste des clients en JSON</t>
+  </si>
+  <si>
+    <t>3) affichage sur le navigateur</t>
+  </si>
+  <si>
+    <t>4) en fonction du conseiller logé, afficher la liste de clients associés</t>
+  </si>
+  <si>
+    <t>1) webservice recupere la liste de clients du conseiller</t>
+  </si>
+  <si>
+    <t>3) afficher sur le navigateur</t>
+  </si>
+  <si>
+    <t>3) affichage du JSON sur le naviguateur</t>
+  </si>
+  <si>
+    <t>4) afficher ses comptes sur une page</t>
+  </si>
+  <si>
+    <t>1) recupérer ses comptes (webservice)</t>
+  </si>
+  <si>
+    <t>2) trier les comptes recus par id du client</t>
+  </si>
+  <si>
+    <t>2) trier avec un id client</t>
+  </si>
+  <si>
+    <t>1) Récupérer la liste des comptes de l'agence via WS</t>
+  </si>
+  <si>
+    <t>Estimation total (back + front)</t>
+  </si>
+  <si>
+    <t>Estimation back</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -431,7 +469,7 @@
     <numFmt numFmtId="164" formatCode="ddd\ dd/mm"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,6 +550,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -551,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1002,6 +1056,15 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1063,7 +1126,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1296,11 +1359,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1384,112 +1459,139 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="55">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -1732,7 +1834,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1778,6 +1880,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1822,25 +1944,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1852,25 +1974,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>116.0</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96.66666666666667</c:v>
+                  <c:v>96.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.33333333333334</c:v>
+                  <c:v>77.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.66666666666667</c:v>
+                  <c:v>38.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.33333333333334</c:v>
+                  <c:v>19.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1914,25 +2036,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1944,25 +2066,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>116.0</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.0</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1979,11 +2101,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2115499912"/>
-        <c:axId val="-2096496680"/>
+        <c:axId val="100978352"/>
+        <c:axId val="100978912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2115499912"/>
+        <c:axId val="100978352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,6 +2146,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2059,10 +2201,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096496680"/>
+        <c:crossAx val="100978912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2070,7 +2212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096496680"/>
+        <c:axId val="100978912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,6 +2267,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2154,11 +2316,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115499912"/>
-        <c:crossesAt val="1.0"/>
+        <c:crossAx val="100978352"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2197,7 +2359,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2227,7 +2389,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2241,7 +2403,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2273,7 +2435,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Burn Down Chart Sprint 0</a:t>
+              <a:t>Burn Down Chart Sprint 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2287,6 +2449,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2331,55 +2513,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$E$31:$K$31</c:f>
+              <c:f>'Sprint 1'!$F$31:$L$31</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>61.0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.83333333333334</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.66666666666667</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.33333333333334</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.16666666666667</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2423,55 +2605,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$E$30:$K$30</c:f>
+              <c:f>'Sprint 1'!$F$30:$L$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>61.0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2488,11 +2670,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136117896"/>
-        <c:axId val="-2114953192"/>
+        <c:axId val="100981712"/>
+        <c:axId val="100982272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2136117896"/>
+        <c:axId val="100981712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,6 +2715,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2568,10 +2770,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114953192"/>
+        <c:crossAx val="100982272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2579,7 +2781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114953192"/>
+        <c:axId val="100982272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2634,6 +2836,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2663,11 +2885,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136117896"/>
-        <c:crossesAt val="1.0"/>
+        <c:crossAx val="100981712"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2706,7 +2928,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2736,7 +2958,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3872,16 +4094,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>479425</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>193675</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4248,29 +4470,29 @@
   <dimension ref="B2:L37"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="62.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="16" thickBot="1"/>
+    <row r="2" spans="2:12" ht="16.5" thickBot="1"/>
     <row r="3" spans="2:12" ht="15" customHeight="1">
-      <c r="B3" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
+      <c r="B3" s="84" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -4278,12 +4500,12 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="2:12" ht="16" thickBot="1">
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="86"/>
+    <row r="4" spans="2:12" ht="16.5" thickBot="1">
+      <c r="B4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -4291,8 +4513,8 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="2:12" ht="16" thickBot="1"/>
-    <row r="6" spans="2:12" ht="16" thickBot="1">
+    <row r="5" spans="2:12" ht="16.5" thickBot="1"/>
+    <row r="6" spans="2:12" ht="16.5" thickBot="1">
       <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
@@ -4321,7 +4543,7 @@
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="90" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -4335,7 +4557,7 @@
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="88"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -4347,7 +4569,7 @@
       </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="88"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
@@ -4385,17 +4607,17 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="2:12" ht="16" thickBot="1">
+    <row r="14" spans="2:12" ht="16.5" thickBot="1">
       <c r="B14" s="59"/>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
     </row>
-    <row r="15" spans="2:12" ht="16" thickBot="1">
+    <row r="15" spans="2:12" ht="16.5" thickBot="1">
       <c r="B15" s="61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="23" customHeight="1" thickBot="1">
+    <row r="16" spans="2:12" ht="23.1" customHeight="1" thickBot="1">
       <c r="B16" s="63" t="s">
         <v>18</v>
       </c>
@@ -4412,7 +4634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="23" customHeight="1">
+    <row r="17" spans="2:6" ht="23.1" customHeight="1">
       <c r="B17" s="62">
         <v>3</v>
       </c>
@@ -4423,11 +4645,11 @@
         <v>100</v>
       </c>
       <c r="E17" s="62">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F17" s="62"/>
     </row>
-    <row r="18" spans="2:6" ht="23" customHeight="1">
+    <row r="18" spans="2:6" ht="23.1" customHeight="1">
       <c r="B18" s="74">
         <v>4</v>
       </c>
@@ -4438,11 +4660,11 @@
         <v>100</v>
       </c>
       <c r="E18" s="74">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F18" s="74"/>
     </row>
-    <row r="19" spans="2:6" ht="23" customHeight="1">
+    <row r="19" spans="2:6" ht="23.1" customHeight="1">
       <c r="B19" s="6">
         <v>6</v>
       </c>
@@ -4457,7 +4679,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="2:6" ht="23" customHeight="1">
+    <row r="20" spans="2:6" ht="23.1" customHeight="1">
       <c r="B20" s="6">
         <v>11</v>
       </c>
@@ -4472,7 +4694,7 @@
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="2:6" ht="23" customHeight="1">
+    <row r="21" spans="2:6" ht="23.1" customHeight="1">
       <c r="B21" s="6">
         <v>10</v>
       </c>
@@ -4483,11 +4705,11 @@
         <v>40</v>
       </c>
       <c r="E21" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="2:6" ht="23" customHeight="1">
+    <row r="22" spans="2:6" ht="23.1" customHeight="1">
       <c r="B22" s="6">
         <v>2</v>
       </c>
@@ -4502,7 +4724,7 @@
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="2:6" ht="23" customHeight="1">
+    <row r="23" spans="2:6" ht="23.1" customHeight="1">
       <c r="B23" s="74">
         <v>1</v>
       </c>
@@ -4517,7 +4739,7 @@
       </c>
       <c r="F23" s="74"/>
     </row>
-    <row r="24" spans="2:6" ht="23" customHeight="1">
+    <row r="24" spans="2:6" ht="23.1" customHeight="1">
       <c r="B24" s="6">
         <v>5</v>
       </c>
@@ -4532,12 +4754,12 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="2:6" ht="23" customHeight="1">
+    <row r="25" spans="2:6" ht="23.1" customHeight="1">
       <c r="B25" s="6">
         <v>9</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D25" s="6">
         <v>20</v>
@@ -4547,12 +4769,12 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="2:6" ht="23" customHeight="1">
+    <row r="26" spans="2:6" ht="23.1" customHeight="1">
       <c r="B26" s="6">
         <v>12</v>
       </c>
       <c r="C26" s="74" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D26" s="6">
         <v>20</v>
@@ -4562,7 +4784,7 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="2:6" ht="23" customHeight="1">
+    <row r="27" spans="2:6" ht="23.1" customHeight="1">
       <c r="B27" s="6">
         <v>13</v>
       </c>
@@ -4577,7 +4799,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:6" ht="23" customHeight="1">
+    <row r="28" spans="2:6" ht="23.1" customHeight="1">
       <c r="B28" s="6">
         <v>7</v>
       </c>
@@ -4592,7 +4814,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="2:6" ht="23" customHeight="1">
+    <row r="29" spans="2:6" ht="23.1" customHeight="1">
       <c r="B29" s="6">
         <v>8</v>
       </c>
@@ -4607,19 +4829,19 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="2:6" ht="23" customHeight="1" thickBot="1">
+    <row r="30" spans="2:6" ht="23.1" customHeight="1" thickBot="1">
       <c r="B30" s="60"/>
       <c r="C30" s="60"/>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
     </row>
-    <row r="31" spans="2:6" ht="16" thickBot="1">
+    <row r="31" spans="2:6" ht="16.5" thickBot="1">
       <c r="B31" s="66" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="16" thickBot="1">
+    <row r="32" spans="2:6" ht="16.5" thickBot="1">
       <c r="B32" s="64" t="s">
         <v>18</v>
       </c>
@@ -4741,17 +4963,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4766,10 +4988,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="89">
+      <c r="A2" s="92">
         <v>1</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="92" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="73" t="s">
@@ -4777,359 +4999,380 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="89"/>
-      <c r="B3" s="89"/>
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="73" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="89"/>
-      <c r="B4" s="89"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="73" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="89"/>
-      <c r="B5" s="89"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="92"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="73" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="93">
+        <v>2</v>
+      </c>
+      <c r="B7" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="72" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="90">
-        <v>2</v>
-      </c>
-      <c r="B6" s="90" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="72" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="93"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="72" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="72" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="93"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="72" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="72" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="92">
+        <v>3</v>
+      </c>
+      <c r="B10" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="92"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="92"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="73" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="92"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="73" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="93">
+        <v>4</v>
+      </c>
+      <c r="B14" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="72" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="89">
-        <v>3</v>
-      </c>
-      <c r="B9" s="89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="73" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="93"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="89"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="73" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="93"/>
+      <c r="B16" s="93"/>
+      <c r="C16" s="72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="93"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="92">
+        <v>5</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="73" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="89"/>
-      <c r="B11" s="89"/>
-      <c r="C11" s="73" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="73" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="90">
-        <v>4</v>
-      </c>
-      <c r="B12" s="90" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="72" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="90"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="72" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="92"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="73" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="90"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="72" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="93">
+        <v>6</v>
+      </c>
+      <c r="B22" s="93" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="72" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="89">
-        <v>5</v>
-      </c>
-      <c r="B15" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="73" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="93"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="93"/>
+      <c r="B24" s="93"/>
+      <c r="C24" s="72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="93"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="72" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="93"/>
+      <c r="B26" s="93"/>
+      <c r="C26" s="72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="93"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="72" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="92">
+        <v>7</v>
+      </c>
+      <c r="B28" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="73" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="73" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="92"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="73" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="89"/>
-      <c r="B17" s="89"/>
-      <c r="C17" s="73" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="92"/>
+      <c r="B30" s="92"/>
+      <c r="C30" s="73" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="89"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="73" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="92"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="73" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="90">
-        <v>6</v>
-      </c>
-      <c r="B19" s="90" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="72" t="s">
+    <row r="32" spans="1:3">
+      <c r="A32" s="92"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="73" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="90"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="72" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="90"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="90"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="72" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="90"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="72" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="90"/>
-      <c r="B24" s="90"/>
-      <c r="C24" s="72" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="89">
-        <v>7</v>
-      </c>
-      <c r="B25" s="89" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="73" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="6">
+        <v>8</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="72" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="89"/>
-      <c r="B26" s="89"/>
-      <c r="C26" s="73" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="92">
+        <v>9</v>
+      </c>
+      <c r="B34" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="89"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="73" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="92"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="73" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="89"/>
-      <c r="B28" s="89"/>
-      <c r="C28" s="73" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="92"/>
+      <c r="B36" s="92"/>
+      <c r="C36" s="73" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="89"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="73" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="93">
+        <v>10</v>
+      </c>
+      <c r="B37" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="72" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="6">
-        <v>8</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="72" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="93"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="72" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="89">
-        <v>9</v>
-      </c>
-      <c r="B31" s="89" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="73" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="92">
+        <v>11</v>
+      </c>
+      <c r="B39" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="73" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="89"/>
-      <c r="B32" s="89"/>
-      <c r="C32" s="73" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="92"/>
+      <c r="B40" s="92"/>
+      <c r="C40" s="73" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="93">
+        <v>12</v>
+      </c>
+      <c r="B41" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="72" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="89"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="73" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" s="93"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="72" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="90">
-        <v>10</v>
-      </c>
-      <c r="B34" s="90" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="72" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="92">
+        <v>13</v>
+      </c>
+      <c r="B43" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="73" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="90"/>
-      <c r="B35" s="90"/>
-      <c r="C35" s="72" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" s="92"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="73" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="89">
-        <v>11</v>
-      </c>
-      <c r="B36" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="73" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="92"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="73" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="89"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="73" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="90">
-        <v>12</v>
-      </c>
-      <c r="B38" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="72" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="90"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="72" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="89">
-        <v>13</v>
-      </c>
-      <c r="B40" s="89" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="73" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="89"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="73" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="89"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="73" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5145,30 +5388,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
+    <col min="1" max="2" width="13.375" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="22"/>
@@ -5238,7 +5481,7 @@
       <c r="K5" s="24"/>
       <c r="M5" s="21"/>
     </row>
-    <row r="6" spans="1:13" ht="16" thickBot="1">
+    <row r="6" spans="1:13" ht="16.5" thickBot="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -5252,23 +5495,23 @@
       <c r="K6" s="24"/>
       <c r="M6" s="21"/>
     </row>
-    <row r="7" spans="1:13" ht="16" thickBot="1">
+    <row r="7" spans="1:13" ht="16.5" thickBot="1">
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="D7" s="34"/>
       <c r="E7" s="33"/>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="102"/>
       <c r="M7" s="21"/>
     </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1">
+    <row r="8" spans="1:13" ht="16.5" thickBot="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -5296,7 +5539,7 @@
       </c>
       <c r="M8" s="21"/>
     </row>
-    <row r="9" spans="1:13" ht="30">
+    <row r="9" spans="1:13" ht="31.5">
       <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
@@ -5316,41 +5559,41 @@
         <v>76</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H9" s="52" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="52" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J9" s="52" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K9" s="52" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="100" t="s">
+      <c r="A10" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-    </row>
-    <row r="11" spans="1:13" ht="45">
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.5">
       <c r="A11" s="35">
         <v>14</v>
       </c>
-      <c r="B11" s="91">
+      <c r="B11" s="94">
         <v>8</v>
       </c>
       <c r="C11" s="36">
@@ -5381,11 +5624,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30">
+    <row r="12" spans="1:13" ht="31.5">
       <c r="A12" s="35">
         <v>14</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="36">
         <v>2</v>
       </c>
@@ -5414,11 +5657,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60">
+    <row r="13" spans="1:13" ht="63">
       <c r="A13" s="35">
         <v>14</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="96"/>
       <c r="C13" s="36">
         <v>3</v>
       </c>
@@ -5448,25 +5691,25 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-    </row>
-    <row r="15" spans="1:13" ht="45">
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+    </row>
+    <row r="15" spans="1:13" ht="47.25">
       <c r="A15" s="35">
         <v>15</v>
       </c>
-      <c r="B15" s="91">
+      <c r="B15" s="94">
         <v>20</v>
       </c>
       <c r="C15" s="36">
@@ -5497,11 +5740,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45">
+    <row r="16" spans="1:13" ht="47.25">
       <c r="A16" s="35">
         <v>15</v>
       </c>
-      <c r="B16" s="92"/>
+      <c r="B16" s="95"/>
       <c r="C16" s="36">
         <v>2</v>
       </c>
@@ -5530,11 +5773,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30">
+    <row r="17" spans="1:11" ht="31.5">
       <c r="A17" s="35">
         <v>15</v>
       </c>
-      <c r="B17" s="92"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="36">
         <v>3</v>
       </c>
@@ -5563,11 +5806,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="60">
+    <row r="18" spans="1:11" ht="63">
       <c r="A18" s="35">
         <v>15</v>
       </c>
-      <c r="B18" s="93"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="36">
         <v>4</v>
       </c>
@@ -5597,25 +5840,25 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="101"/>
-      <c r="J19" s="101"/>
-      <c r="K19" s="101"/>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+    </row>
+    <row r="20" spans="1:11" ht="47.25">
       <c r="A20" s="35">
         <v>17</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B20" s="106">
         <v>8</v>
       </c>
       <c r="C20" s="35">
@@ -5646,11 +5889,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30">
+    <row r="21" spans="1:11" ht="31.5">
       <c r="A21" s="35">
         <v>17</v>
       </c>
-      <c r="B21" s="104"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="35">
         <v>2</v>
       </c>
@@ -5679,11 +5922,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="60">
+    <row r="22" spans="1:11" ht="63">
       <c r="A22" s="35">
         <v>17</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="108"/>
       <c r="C22" s="35">
         <v>3</v>
       </c>
@@ -5713,25 +5956,25 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="102" t="s">
+      <c r="A23" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="101"/>
-    </row>
-    <row r="24" spans="1:11" ht="45">
+      <c r="B23" s="104"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+    </row>
+    <row r="24" spans="1:11" ht="47.25">
       <c r="A24" s="35">
         <v>16</v>
       </c>
-      <c r="B24" s="91">
+      <c r="B24" s="94">
         <v>40</v>
       </c>
       <c r="C24" s="36">
@@ -5762,11 +6005,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="60">
+    <row r="25" spans="1:11" ht="63">
       <c r="A25" s="35">
         <v>16</v>
       </c>
-      <c r="B25" s="92"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="36">
         <v>2</v>
       </c>
@@ -5795,11 +6038,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="60">
+    <row r="26" spans="1:11" ht="63">
       <c r="A26" s="35">
         <v>16</v>
       </c>
-      <c r="B26" s="93"/>
+      <c r="B26" s="96"/>
       <c r="C26" s="36">
         <v>3</v>
       </c>
@@ -5829,25 +6072,25 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="102" t="s">
+      <c r="A27" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+      <c r="B27" s="104"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="104"/>
+    </row>
+    <row r="28" spans="1:11" ht="31.5">
       <c r="A28" s="35">
         <v>18</v>
       </c>
-      <c r="B28" s="91">
+      <c r="B28" s="94">
         <v>40</v>
       </c>
       <c r="C28" s="36">
@@ -5878,11 +6121,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30">
+    <row r="29" spans="1:11" ht="31.5">
       <c r="A29" s="35">
         <v>18</v>
       </c>
-      <c r="B29" s="92"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="36">
         <v>2</v>
       </c>
@@ -5911,11 +6154,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45">
+    <row r="30" spans="1:11" ht="47.25">
       <c r="A30" s="35">
         <v>18</v>
       </c>
-      <c r="B30" s="92"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="36">
         <v>3</v>
       </c>
@@ -5944,11 +6187,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45">
+    <row r="31" spans="1:11" ht="47.25">
       <c r="A31" s="35">
         <v>18</v>
       </c>
-      <c r="B31" s="92"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="36">
         <v>4</v>
       </c>
@@ -5977,11 +6220,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30">
+    <row r="32" spans="1:11" ht="31.5">
       <c r="A32" s="35">
         <v>18</v>
       </c>
-      <c r="B32" s="93"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="36">
         <v>5</v>
       </c>
@@ -6010,7 +6253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="30">
+    <row r="33" spans="1:13" ht="31.5">
       <c r="A33" s="33"/>
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
@@ -6047,7 +6290,7 @@
       </c>
       <c r="M33" s="21"/>
     </row>
-    <row r="34" spans="1:13" ht="45">
+    <row r="34" spans="1:13" ht="47.25">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -6133,491 +6376,516 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="80.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="80.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="94" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-    </row>
-    <row r="2" spans="1:13">
+    <row r="1" spans="1:14">
+      <c r="A1" s="129" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
-      <c r="M2" s="21"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="L2" s="24"/>
+      <c r="N2" s="21"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="46" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="F3" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="27"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
       <c r="K3" s="27"/>
-      <c r="M3" s="21"/>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="L3" s="27"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="25">
+      <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
-      <c r="M4" s="21"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="L4" s="24"/>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="28">
+      <c r="F5" s="28">
         <v>43109</v>
       </c>
-      <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
-      <c r="M5" s="21"/>
-    </row>
-    <row r="6" spans="1:13" ht="16" thickBot="1">
+      <c r="L5" s="24"/>
+      <c r="N5" s="21"/>
+    </row>
+    <row r="6" spans="1:14" ht="16.5" thickBot="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" ht="16" thickBot="1">
+      <c r="L6" s="24"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" ht="16.5" thickBot="1">
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="97" t="s">
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1">
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="102"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="1:14" ht="16.5" thickBot="1">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="75">
-        <v>0</v>
-      </c>
-      <c r="F8" s="76">
+      <c r="D8" s="33"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="75">
+        <v>0</v>
+      </c>
+      <c r="G8" s="76">
         <v>1</v>
       </c>
-      <c r="G8" s="76">
+      <c r="H8" s="76">
         <v>2</v>
       </c>
-      <c r="H8" s="76">
+      <c r="I8" s="76">
         <v>3</v>
       </c>
-      <c r="I8" s="76">
+      <c r="J8" s="76">
         <v>4</v>
       </c>
-      <c r="J8" s="76">
+      <c r="K8" s="76">
         <v>5</v>
       </c>
-      <c r="K8" s="77">
+      <c r="L8" s="77">
         <v>6</v>
       </c>
-      <c r="M8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" ht="30">
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="1:14" ht="47.25">
       <c r="A9" s="48" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="E9" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="F9" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="52" t="s">
-        <v>121</v>
-      </c>
       <c r="G9" s="52" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="H9" s="52" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I9" s="52" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J9" s="52" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K9" s="52" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="100" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="108">
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="106">
         <v>3</v>
       </c>
-      <c r="B11" s="107">
+      <c r="B11" s="106">
+        <v>13</v>
+      </c>
+      <c r="C11" s="106">
+        <v>9</v>
+      </c>
+      <c r="D11" s="79">
+        <v>1</v>
+      </c>
+      <c r="E11" s="122" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="40">
         <v>3</v>
       </c>
-      <c r="C11" s="80">
-        <v>1</v>
-      </c>
-      <c r="D11" s="118" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="40">
-        <v>1</v>
-      </c>
-      <c r="F11" s="80">
-        <v>1</v>
-      </c>
-      <c r="G11" s="35">
-        <v>1</v>
+      <c r="G11" s="79">
+        <v>2</v>
       </c>
       <c r="H11" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K11" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="109"/>
+        <v>3</v>
+      </c>
+      <c r="L11" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="107"/>
       <c r="B12" s="107"/>
-      <c r="C12" s="80">
+      <c r="C12" s="107"/>
+      <c r="D12" s="79">
         <v>2</v>
       </c>
-      <c r="D12" s="118" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="40">
-        <v>1</v>
-      </c>
-      <c r="F12" s="80">
-        <v>0</v>
-      </c>
-      <c r="G12" s="78">
-        <v>1</v>
+      <c r="E12" s="122" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" s="40">
+        <v>5</v>
+      </c>
+      <c r="G12" s="79">
+        <v>0</v>
       </c>
       <c r="H12" s="78">
         <v>1</v>
       </c>
       <c r="I12" s="78">
+        <v>4</v>
+      </c>
+      <c r="J12" s="78">
+        <v>5</v>
+      </c>
+      <c r="K12" s="78">
+        <v>5</v>
+      </c>
+      <c r="L12" s="78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="107"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="108"/>
+      <c r="D13" s="79">
+        <v>3</v>
+      </c>
+      <c r="E13" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="F13" s="40">
         <v>1</v>
       </c>
-      <c r="J12" s="78">
+      <c r="G13" s="79">
+        <v>0</v>
+      </c>
+      <c r="H13" s="35">
+        <v>0</v>
+      </c>
+      <c r="I13" s="35">
+        <v>0</v>
+      </c>
+      <c r="J13" s="35">
+        <v>0</v>
+      </c>
+      <c r="K13" s="35">
+        <v>0</v>
+      </c>
+      <c r="L13" s="35">
         <v>1</v>
       </c>
-      <c r="K12" s="78">
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="119"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="116">
+        <v>4</v>
+      </c>
+      <c r="B15" s="111">
+        <v>20</v>
+      </c>
+      <c r="C15" s="106">
+        <v>14</v>
+      </c>
+      <c r="D15" s="79">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="110"/>
-      <c r="B13" s="107"/>
-      <c r="C13" s="80">
+      <c r="E15" s="123" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="40">
+        <v>4</v>
+      </c>
+      <c r="G15" s="83">
+        <v>4</v>
+      </c>
+      <c r="H15" s="39">
+        <v>4</v>
+      </c>
+      <c r="I15" s="39">
+        <v>4</v>
+      </c>
+      <c r="J15" s="39">
+        <v>4</v>
+      </c>
+      <c r="K15" s="39">
+        <v>4</v>
+      </c>
+      <c r="L15" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="117"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="79">
+        <v>2</v>
+      </c>
+      <c r="E16" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="40">
+        <v>8</v>
+      </c>
+      <c r="G16" s="120">
+        <v>0</v>
+      </c>
+      <c r="H16" s="80">
+        <v>2</v>
+      </c>
+      <c r="I16" s="121">
+        <v>4</v>
+      </c>
+      <c r="J16" s="121">
+        <v>2</v>
+      </c>
+      <c r="K16" s="121">
+        <v>8</v>
+      </c>
+      <c r="L16" s="121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="118"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="79">
         <v>3</v>
       </c>
-      <c r="D13" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="40">
+      <c r="E17" s="123" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="40">
+        <v>2</v>
+      </c>
+      <c r="G17" s="83">
+        <v>0</v>
+      </c>
+      <c r="H17" s="39">
+        <v>0</v>
+      </c>
+      <c r="I17" s="39">
+        <v>0</v>
+      </c>
+      <c r="J17" s="39">
+        <v>0</v>
+      </c>
+      <c r="K17" s="39">
+        <v>0</v>
+      </c>
+      <c r="L17" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="119"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="104"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="112">
+        <v>6</v>
+      </c>
+      <c r="B19" s="106">
+        <v>40</v>
+      </c>
+      <c r="C19" s="106">
+        <v>27</v>
+      </c>
+      <c r="D19" s="81">
         <v>1</v>
       </c>
-      <c r="F13" s="80">
-        <v>0</v>
-      </c>
-      <c r="G13" s="35">
-        <v>0</v>
-      </c>
-      <c r="H13" s="35">
-        <v>1</v>
-      </c>
-      <c r="I13" s="35">
-        <v>1</v>
-      </c>
-      <c r="J13" s="35">
-        <v>1</v>
-      </c>
-      <c r="K13" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="100" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="115"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="117"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="108">
-        <v>4</v>
-      </c>
-      <c r="B15" s="107">
-        <v>8</v>
-      </c>
-      <c r="C15" s="80">
-        <v>1</v>
-      </c>
-      <c r="D15" s="119" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="40">
+      <c r="E19" s="125" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="40">
         <v>3</v>
-      </c>
-      <c r="F15" s="114">
-        <v>0</v>
-      </c>
-      <c r="G15" s="39">
-        <v>1</v>
-      </c>
-      <c r="H15" s="39">
-        <v>1</v>
-      </c>
-      <c r="I15" s="39">
-        <v>3</v>
-      </c>
-      <c r="J15" s="39">
-        <v>3</v>
-      </c>
-      <c r="K15" s="39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="109"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="80">
-        <v>2</v>
-      </c>
-      <c r="D16" s="119" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="40">
-        <v>2</v>
-      </c>
-      <c r="F16" s="114">
-        <v>2</v>
-      </c>
-      <c r="G16" s="39">
-        <v>2</v>
-      </c>
-      <c r="H16" s="39">
-        <v>2</v>
-      </c>
-      <c r="I16" s="39">
-        <v>2</v>
-      </c>
-      <c r="J16" s="39">
-        <v>2</v>
-      </c>
-      <c r="K16" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="110"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="80">
-        <v>3</v>
-      </c>
-      <c r="D17" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="40">
-        <v>3</v>
-      </c>
-      <c r="F17" s="114">
-        <v>0</v>
-      </c>
-      <c r="G17" s="39">
-        <v>0</v>
-      </c>
-      <c r="H17" s="39">
-        <v>3</v>
-      </c>
-      <c r="I17" s="39">
-        <v>3</v>
-      </c>
-      <c r="J17" s="39">
-        <v>3</v>
-      </c>
-      <c r="K17" s="39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="106"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="106"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="101"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="111">
-        <v>6</v>
-      </c>
-      <c r="B19" s="103">
-        <v>40</v>
-      </c>
-      <c r="C19" s="35">
-        <v>1</v>
-      </c>
-      <c r="D19" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" s="40">
-        <v>6</v>
-      </c>
-      <c r="F19" s="39">
-        <v>0</v>
       </c>
       <c r="G19" s="39">
         <v>3</v>
       </c>
       <c r="H19" s="39">
+        <v>3</v>
+      </c>
+      <c r="I19" s="39">
+        <v>3</v>
+      </c>
+      <c r="J19" s="39">
+        <v>3</v>
+      </c>
+      <c r="K19" s="39">
+        <v>3</v>
+      </c>
+      <c r="L19" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="113"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="81">
         <v>2</v>
       </c>
-      <c r="I19" s="39">
-        <v>6</v>
-      </c>
-      <c r="J19" s="39">
-        <v>6</v>
-      </c>
-      <c r="K19" s="39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="112"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="35">
+      <c r="E20" s="127" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="40">
+        <v>4</v>
+      </c>
+      <c r="G20" s="39">
+        <v>1</v>
+      </c>
+      <c r="H20" s="39">
         <v>2</v>
       </c>
-      <c r="D20" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="40">
-        <v>4</v>
-      </c>
-      <c r="F20" s="39">
+      <c r="I20" s="39">
         <v>3</v>
-      </c>
-      <c r="G20" s="39">
-        <v>4</v>
-      </c>
-      <c r="H20" s="39">
-        <v>4</v>
-      </c>
-      <c r="I20" s="39">
-        <v>4</v>
       </c>
       <c r="J20" s="39">
         <v>4</v>
@@ -6625,173 +6893,181 @@
       <c r="K20" s="39">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="112"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="78">
+      <c r="L20" s="39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="113"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="81">
         <v>3</v>
       </c>
-      <c r="D21" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="40">
+      <c r="E21" s="125" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="40">
+        <v>2</v>
+      </c>
+      <c r="G21" s="39">
+        <v>0</v>
+      </c>
+      <c r="H21" s="39">
+        <v>0</v>
+      </c>
+      <c r="I21" s="39">
+        <v>2</v>
+      </c>
+      <c r="J21" s="39">
+        <v>2</v>
+      </c>
+      <c r="K21" s="39">
+        <v>2</v>
+      </c>
+      <c r="L21" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="113"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="81">
+        <v>4</v>
+      </c>
+      <c r="E22" s="125" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="40">
+        <v>9</v>
+      </c>
+      <c r="G22" s="39">
+        <v>0</v>
+      </c>
+      <c r="H22" s="39">
+        <v>0</v>
+      </c>
+      <c r="I22" s="39">
+        <v>1</v>
+      </c>
+      <c r="J22" s="39">
+        <v>5</v>
+      </c>
+      <c r="K22" s="39">
+        <v>8</v>
+      </c>
+      <c r="L22" s="39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="113"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="107"/>
+      <c r="D23" s="81">
+        <v>5</v>
+      </c>
+      <c r="E23" s="125" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="40">
+        <v>7</v>
+      </c>
+      <c r="G23" s="39">
+        <v>0</v>
+      </c>
+      <c r="H23" s="39">
+        <v>0</v>
+      </c>
+      <c r="I23" s="39">
+        <v>0</v>
+      </c>
+      <c r="J23" s="39">
+        <v>0</v>
+      </c>
+      <c r="K23" s="39">
+        <v>2</v>
+      </c>
+      <c r="L23" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="114"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="81">
         <v>6</v>
       </c>
-      <c r="F21" s="39">
+      <c r="E24" s="125" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="40">
         <v>2</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G24" s="39">
+        <v>0</v>
+      </c>
+      <c r="H24" s="39">
+        <v>0</v>
+      </c>
+      <c r="I24" s="39">
+        <v>0</v>
+      </c>
+      <c r="J24" s="39">
+        <v>0</v>
+      </c>
+      <c r="K24" s="39">
+        <v>0</v>
+      </c>
+      <c r="L24" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="115"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="104"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="82">
+        <v>11</v>
+      </c>
+      <c r="B26" s="81">
+        <v>100</v>
+      </c>
+      <c r="C26" s="79">
+        <v>10</v>
+      </c>
+      <c r="D26" s="79">
+        <v>1</v>
+      </c>
+      <c r="E26" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="40">
+        <v>10</v>
+      </c>
+      <c r="G26" s="83">
+        <v>2</v>
+      </c>
+      <c r="H26" s="39">
         <v>3</v>
       </c>
-      <c r="H21" s="39">
+      <c r="I26" s="39">
         <v>6</v>
-      </c>
-      <c r="I21" s="39">
-        <v>6</v>
-      </c>
-      <c r="J21" s="39">
-        <v>6</v>
-      </c>
-      <c r="K21" s="39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="112"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="78">
-        <v>4</v>
-      </c>
-      <c r="D22" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="40">
-        <v>15</v>
-      </c>
-      <c r="F22" s="39">
-        <v>0</v>
-      </c>
-      <c r="G22" s="39">
-        <v>0</v>
-      </c>
-      <c r="H22" s="39">
-        <v>3</v>
-      </c>
-      <c r="I22" s="39">
-        <v>8</v>
-      </c>
-      <c r="J22" s="39">
-        <v>12</v>
-      </c>
-      <c r="K22" s="39">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="112"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="78">
-        <v>5</v>
-      </c>
-      <c r="D23" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="40">
-        <v>7</v>
-      </c>
-      <c r="F23" s="39">
-        <v>0</v>
-      </c>
-      <c r="G23" s="39">
-        <v>0</v>
-      </c>
-      <c r="H23" s="39">
-        <v>0</v>
-      </c>
-      <c r="I23" s="39">
-        <v>0</v>
-      </c>
-      <c r="J23" s="39">
-        <v>2</v>
-      </c>
-      <c r="K23" s="39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="113"/>
-      <c r="B24" s="105"/>
-      <c r="C24" s="78">
-        <v>6</v>
-      </c>
-      <c r="D24" s="72" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="40">
-        <v>2</v>
-      </c>
-      <c r="F24" s="39">
-        <v>0</v>
-      </c>
-      <c r="G24" s="39">
-        <v>0</v>
-      </c>
-      <c r="H24" s="39">
-        <v>0</v>
-      </c>
-      <c r="I24" s="39">
-        <v>0</v>
-      </c>
-      <c r="J24" s="39">
-        <v>0</v>
-      </c>
-      <c r="K24" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="102" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="115"/>
-      <c r="C25" s="101"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="115"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="101"/>
-      <c r="I25" s="101"/>
-      <c r="J25" s="101"/>
-      <c r="K25" s="101"/>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="79">
-        <v>11</v>
-      </c>
-      <c r="B26" s="78">
-        <v>100</v>
-      </c>
-      <c r="C26" s="80">
-        <v>1</v>
-      </c>
-      <c r="D26" s="118" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="40">
-        <v>10</v>
-      </c>
-      <c r="F26" s="114">
-        <v>2</v>
-      </c>
-      <c r="G26" s="39">
-        <v>3</v>
-      </c>
-      <c r="H26" s="39">
-        <v>6</v>
-      </c>
-      <c r="I26" s="39">
-        <v>10</v>
       </c>
       <c r="J26" s="39">
         <v>10</v>
@@ -6799,43 +7075,47 @@
       <c r="K26" s="39">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="116" t="s">
+      <c r="L26" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="109" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="101"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="M27" s="21"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="107">
+      <c r="B27" s="110"/>
+      <c r="C27" s="110"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="104"/>
+      <c r="N27" s="21"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="111">
         <v>10</v>
       </c>
-      <c r="B28" s="107">
+      <c r="B28" s="111">
+        <v>5</v>
+      </c>
+      <c r="C28" s="106">
         <v>3</v>
       </c>
-      <c r="C28" s="80">
+      <c r="D28" s="79">
         <v>1</v>
       </c>
-      <c r="D28" s="119" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="40">
+      <c r="E28" s="123" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="40">
         <v>2</v>
       </c>
-      <c r="F28" s="114">
-        <v>2</v>
-      </c>
-      <c r="G28" s="39">
+      <c r="G28" s="83">
         <v>2</v>
       </c>
       <c r="H28" s="39">
@@ -6850,25 +7130,26 @@
       <c r="K28" s="39">
         <v>2</v>
       </c>
-      <c r="M28" s="21"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="107"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="80">
+      <c r="L28" s="39">
         <v>2</v>
       </c>
-      <c r="D29" s="119" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="40">
+      <c r="N28" s="21"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="111"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="79">
+        <v>2</v>
+      </c>
+      <c r="E29" s="123" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="40">
         <v>1</v>
       </c>
-      <c r="F29" s="114">
-        <v>0</v>
-      </c>
-      <c r="G29" s="39">
-        <v>1</v>
+      <c r="G29" s="83">
+        <v>0</v>
       </c>
       <c r="H29" s="39">
         <v>1</v>
@@ -6882,108 +7163,125 @@
       <c r="K29" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="D30" s="56" t="s">
+      <c r="L29" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="128" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="121">
+        <f>SUM(B11,B15,B19,B26,B28)</f>
+        <v>178</v>
+      </c>
+      <c r="C30" s="121">
+        <f>SUM(C11,C15,C19,C26,C28)</f>
+        <v>63</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="41">
-        <f>SUM(E11:E26)</f>
-        <v>61</v>
-      </c>
       <c r="F30" s="41">
-        <f>$E30-SUM(F11:F26)</f>
-        <v>51</v>
+        <f>SUM(F11:F29)</f>
+        <v>63</v>
       </c>
       <c r="G30" s="41">
-        <f>$E30-SUM(G11:G26)</f>
-        <v>43</v>
+        <f>$F30-SUM(G11:G29)</f>
+        <v>49</v>
       </c>
       <c r="H30" s="41">
-        <f>$E30-SUM(H11:H26)</f>
-        <v>31</v>
+        <f>$F30-SUM(H11:H29)</f>
+        <v>42</v>
       </c>
       <c r="I30" s="41">
-        <f>$E30-SUM(I11:I26)</f>
-        <v>16</v>
+        <f>$F30-SUM(I11:I29)</f>
+        <v>30</v>
       </c>
       <c r="J30" s="41">
-        <f>$E30-SUM(J11:J26)</f>
-        <v>10</v>
+        <f>$F30-SUM(J11:J29)</f>
+        <v>22</v>
       </c>
       <c r="K30" s="41">
-        <f>$E30-SUM(K11:K26)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="D31" s="57" t="s">
+        <f>$F30-SUM(K11:K29)</f>
+        <v>11</v>
+      </c>
+      <c r="L30" s="41">
+        <f>$F30-SUM(L11:L29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="45"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="26">
-        <f>SUM(E11:E26)</f>
-        <v>61</v>
-      </c>
-      <c r="F31" s="42">
-        <f>-(E31/K8)*F8+E31</f>
-        <v>50.833333333333336</v>
+      <c r="F31" s="26">
+        <f>SUM(F11:F29)</f>
+        <v>63</v>
       </c>
       <c r="G31" s="42">
-        <f>-($E31/$K8)*G8+$E31</f>
-        <v>40.666666666666671</v>
+        <f>-(F31/L8)*G8+F31</f>
+        <v>52.5</v>
       </c>
       <c r="H31" s="42">
-        <f>-($E31/$K8)*H8+$E31</f>
-        <v>30.5</v>
+        <f>-($F31/$L8)*H8+$F31</f>
+        <v>42</v>
       </c>
       <c r="I31" s="42">
-        <f>-($E31/$K8)*I8+$E31</f>
-        <v>20.333333333333336</v>
+        <f>-($F31/$L8)*I8+$F31</f>
+        <v>31.5</v>
       </c>
       <c r="J31" s="42">
-        <f>-($E31/$K8)*J8+$E31</f>
-        <v>10.166666666666671</v>
+        <f>-($F31/$L8)*J8+$F31</f>
+        <v>21</v>
       </c>
       <c r="K31" s="42">
-        <f>-($E31/$K8)*K8+$E31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5">
-      <c r="E34">
-        <f>SUM(E19:E24)</f>
-        <v>40</v>
+        <f>-($F31/$L8)*K8+$F31</f>
+        <v>10.5</v>
+      </c>
+      <c r="L31" s="42">
+        <f>-($F31/$L8)*L8+$F31</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A27:K27"/>
+  <mergeCells count="19">
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A27:L27"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="B19:B24"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:K18"/>
-    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="F30:K30">
+  <conditionalFormatting sqref="G30:L30">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
-      <formula>F31</formula>
+      <formula>G31</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
-      <formula>F31</formula>
+      <formula>G31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>